<commit_message>
reworking the data split and model training. the best result so far.
</commit_message>
<xml_diff>
--- a/y_prediction.xlsx
+++ b/y_prediction.xlsx
@@ -390,7 +390,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10.7340784072876</v>
+        <v>13.8809986114502</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -398,7 +398,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>11.3854455947876</v>
+        <v>7.95662784576416</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -406,7 +406,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7.717073917388916</v>
+        <v>5.955420017242432</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -414,7 +414,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>12.12401676177979</v>
+        <v>6.767120838165283</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -422,7 +422,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>13.9938325881958</v>
+        <v>7.603854179382324</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -430,7 +430,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>13.41903209686279</v>
+        <v>11.47830581665039</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -438,7 +438,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>12.38803768157959</v>
+        <v>13.53664112091064</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -446,7 +446,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>9.054262161254883</v>
+        <v>10.49045848846436</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -454,7 +454,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3.922260284423828</v>
+        <v>4.737107753753662</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -462,7 +462,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>10.83757781982422</v>
+        <v>6.079762935638428</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -470,7 +470,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>10.55265140533447</v>
+        <v>4.378615856170654</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -478,7 +478,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5.683326721191406</v>
+        <v>7.389666080474854</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -486,7 +486,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>14.48312664031982</v>
+        <v>10.40564441680908</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -494,7 +494,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>18.16646957397461</v>
+        <v>10.42655563354492</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -502,7 +502,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>14.57286548614502</v>
+        <v>10.09898853302002</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -510,7 +510,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>6.11720609664917</v>
+        <v>6.089284420013428</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -518,7 +518,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>15.56603908538818</v>
+        <v>4.424148559570312</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -526,7 +526,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>16.53540229797363</v>
+        <v>13.29117012023926</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -534,7 +534,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>12.30655670166016</v>
+        <v>19.33496475219727</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -542,7 +542,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>10.94198894500732</v>
+        <v>6.577813625335693</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -550,7 +550,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>11.99962329864502</v>
+        <v>5.151782989501953</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -558,7 +558,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>10.85213470458984</v>
+        <v>4.395680904388428</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -566,7 +566,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>11.28206729888916</v>
+        <v>6.069608688354492</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -574,7 +574,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>6.95817232131958</v>
+        <v>6.620934963226318</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -582,7 +582,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>10.30211162567139</v>
+        <v>7.318948745727539</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -590,7 +590,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>8.785508155822754</v>
+        <v>11.81636333465576</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -598,7 +598,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>15.61180591583252</v>
+        <v>8.639409065246582</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -606,7 +606,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>16.32898330688477</v>
+        <v>11.24605464935303</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -614,7 +614,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>18.95686149597168</v>
+        <v>14.32633876800537</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -622,7 +622,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>14.73952484130859</v>
+        <v>11.50711727142334</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -630,7 +630,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>10.84650421142578</v>
+        <v>15.95943927764893</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -638,7 +638,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>11.24222278594971</v>
+        <v>6.54820442199707</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -646,7 +646,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>13.41308784484863</v>
+        <v>19.80498123168945</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -654,7 +654,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>18.12321472167969</v>
+        <v>25.43582534790039</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -662,7 +662,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>11.22954750061035</v>
+        <v>13.52932548522949</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -670,7 +670,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>11.06840801239014</v>
+        <v>7.902271747589111</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -678,7 +678,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>6.800952911376953</v>
+        <v>6.021476745605469</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -686,7 +686,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>12.38935089111328</v>
+        <v>6.838600158691406</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -694,7 +694,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>13.49728393554688</v>
+        <v>7.617969036102295</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -702,7 +702,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>13.71642017364502</v>
+        <v>11.15285015106201</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -710,7 +710,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>12.49695301055908</v>
+        <v>13.29177665710449</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -718,7 +718,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>9.073392868041992</v>
+        <v>10.23600673675537</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -726,7 +726,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>3.931249856948853</v>
+        <v>4.950057506561279</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -734,7 +734,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>10.58390522003174</v>
+        <v>6.18470287322998</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -742,7 +742,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>10.05390071868896</v>
+        <v>4.31477689743042</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -750,7 +750,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>5.886467933654785</v>
+        <v>7.165870189666748</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -758,7 +758,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>14.71814346313477</v>
+        <v>10.13792991638184</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -766,7 +766,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>17.11821556091309</v>
+        <v>9.974912643432617</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -774,7 +774,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>14.91587448120117</v>
+        <v>9.893525123596191</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -782,7 +782,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>5.580786228179932</v>
+        <v>5.997543811798096</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -790,7 +790,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>15.90250587463379</v>
+        <v>4.566448211669922</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -798,7 +798,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>16.22953796386719</v>
+        <v>12.97424793243408</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -806,7 +806,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>12.79185390472412</v>
+        <v>19.20149993896484</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -814,7 +814,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>10.6183385848999</v>
+        <v>6.523789882659912</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -822,7 +822,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>10.92308521270752</v>
+        <v>5.140477657318115</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -830,7 +830,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>11.40588855743408</v>
+        <v>4.459598064422607</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -838,7 +838,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>10.98503589630127</v>
+        <v>6.025604724884033</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -846,7 +846,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>8.036754608154297</v>
+        <v>6.619915008544922</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -854,7 +854,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>9.096149444580078</v>
+        <v>7.2478346824646</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -862,7 +862,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>9.026552200317383</v>
+        <v>11.04336071014404</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -870,7 +870,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>13.01296901702881</v>
+        <v>8.525527000427246</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -878,7 +878,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>16.67765426635742</v>
+        <v>11.04471969604492</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -886,7 +886,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>16.94958877563477</v>
+        <v>13.73667907714844</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -894,7 +894,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>14.65716552734375</v>
+        <v>11.18331527709961</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -902,7 +902,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>10.64328098297119</v>
+        <v>15.89662742614746</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -910,7 +910,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>9.885561943054199</v>
+        <v>6.532844543457031</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -918,7 +918,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>11.50492763519287</v>
+        <v>19.44545364379883</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -926,7 +926,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>14.7463207244873</v>
+        <v>24.73703193664551</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -934,7 +934,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>11.37626171112061</v>
+        <v>13.4672269821167</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -942,7 +942,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>10.6452054977417</v>
+        <v>7.831560611724854</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -950,7 +950,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>6.689661026000977</v>
+        <v>6.095869064331055</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -958,7 +958,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>12.46042823791504</v>
+        <v>6.864828586578369</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -966,7 +966,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>12.8285961151123</v>
+        <v>7.593636989593506</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -974,7 +974,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>12.78127384185791</v>
+        <v>11.05364608764648</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -982,7 +982,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>12.86518096923828</v>
+        <v>13.05564117431641</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -990,7 +990,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>9.73786735534668</v>
+        <v>10.1266508102417</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -998,7 +998,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>3.945497989654541</v>
+        <v>5.177108287811279</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1006,7 +1006,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>10.1747350692749</v>
+        <v>6.270837306976318</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1014,7 +1014,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>9.004464149475098</v>
+        <v>4.252202033996582</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1022,7 +1022,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>6.28728199005127</v>
+        <v>6.946003913879395</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1030,7 +1030,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>14.43929672241211</v>
+        <v>9.864738464355469</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1038,7 +1038,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>16.1559886932373</v>
+        <v>9.410311698913574</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1046,7 +1046,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>14.886887550354</v>
+        <v>9.71759033203125</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1054,7 +1054,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>5.447003841400146</v>
+        <v>5.906689167022705</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1062,7 +1062,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>13.11125659942627</v>
+        <v>4.805705070495605</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1070,7 +1070,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>16.0885009765625</v>
+        <v>12.64804077148438</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1078,7 +1078,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>12.33454322814941</v>
+        <v>19.15567207336426</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1086,7 +1086,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>10.26038932800293</v>
+        <v>6.473563671112061</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1094,7 +1094,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>10.72667503356934</v>
+        <v>5.091256618499756</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1102,7 +1102,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>11.53893947601318</v>
+        <v>4.499393939971924</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1110,7 +1110,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>10.96871662139893</v>
+        <v>6.052968978881836</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1118,7 +1118,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>8.077991485595703</v>
+        <v>6.607266902923584</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1126,7 +1126,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>8.414040565490723</v>
+        <v>7.175524711608887</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1134,7 +1134,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>9.009664535522461</v>
+        <v>10.60240840911865</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1142,7 +1142,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>11.08544254302979</v>
+        <v>8.40052318572998</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1150,7 +1150,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>16.31133270263672</v>
+        <v>10.70535087585449</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1158,7 +1158,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>14.25123691558838</v>
+        <v>13.24186706542969</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1166,7 +1166,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>13.12438678741455</v>
+        <v>11.0146427154541</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1174,7 +1174,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>10.58473491668701</v>
+        <v>15.82266807556152</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1182,7 +1182,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>9.890063285827637</v>
+        <v>6.48128604888916</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1190,7 +1190,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>10.37007427215576</v>
+        <v>19.08477592468262</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1198,7 +1198,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>12.57071113586426</v>
+        <v>23.96520614624023</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1206,7 +1206,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>11.65828132629395</v>
+        <v>13.74034023284912</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1214,7 +1214,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>10.70360946655273</v>
+        <v>7.841311931610107</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1222,7 +1222,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>6.712057113647461</v>
+        <v>6.168068885803223</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1230,7 +1230,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>12.09603309631348</v>
+        <v>6.835846900939941</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1238,7 +1238,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>12.56362342834473</v>
+        <v>7.528514862060547</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1246,7 +1246,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>10.35196876525879</v>
+        <v>10.78582572937012</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1254,7 +1254,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>12.99033451080322</v>
+        <v>12.74608516693115</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1262,7 +1262,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>10.00134563446045</v>
+        <v>10.11339473724365</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1270,7 +1270,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>4.783513069152832</v>
+        <v>5.427739143371582</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1278,7 +1278,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>9.344485282897949</v>
+        <v>6.331255912780762</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1286,7 +1286,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>7.160605907440186</v>
+        <v>4.204568862915039</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1294,7 +1294,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>6.083680629730225</v>
+        <v>6.737100601196289</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1302,7 +1302,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>13.24258518218994</v>
+        <v>9.57958984375</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1310,7 +1310,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>14.877121925354</v>
+        <v>8.886554718017578</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1318,7 +1318,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>14.22961807250977</v>
+        <v>9.530409812927246</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1326,7 +1326,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>5.194126605987549</v>
+        <v>5.814504623413086</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1334,7 +1334,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>9.39319896697998</v>
+        <v>4.861351013183594</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1342,7 +1342,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>16.03801345825195</v>
+        <v>12.26574897766113</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1350,7 +1350,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>11.40594387054443</v>
+        <v>18.90688514709473</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1358,7 +1358,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>9.984151840209961</v>
+        <v>6.423656940460205</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1366,7 +1366,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>10.68394088745117</v>
+        <v>5.126580238342285</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1374,7 +1374,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>11.44256401062012</v>
+        <v>4.519901275634766</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1382,7 +1382,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>10.64732265472412</v>
+        <v>6.120871543884277</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1390,7 +1390,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>8.018496513366699</v>
+        <v>6.603997707366943</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1398,7 +1398,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>7.80933952331543</v>
+        <v>7.106751918792725</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1406,7 +1406,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>9.583318710327148</v>
+        <v>10.43985939025879</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1414,7 +1414,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>10.55798149108887</v>
+        <v>8.278443336486816</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1422,7 +1422,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>16.01856422424316</v>
+        <v>10.38094711303711</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1430,7 +1430,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>12.27727699279785</v>
+        <v>12.79089641571045</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1438,7 +1438,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>11.76810169219971</v>
+        <v>10.76794719696045</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1446,7 +1446,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>10.54654884338379</v>
+        <v>15.74698162078857</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1454,7 +1454,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>9.898434638977051</v>
+        <v>6.446595668792725</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1462,7 +1462,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>10.56779003143311</v>
+        <v>18.74972724914551</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1470,7 +1470,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>10.96787452697754</v>
+        <v>23.27029037475586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing unsaved changes from previous, training new model with replication, best model obtained. prediction obtained.
</commit_message>
<xml_diff>
--- a/y_prediction.xlsx
+++ b/y_prediction.xlsx
@@ -390,7 +390,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13.8809986114502</v>
+        <v>14.19726943969727</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -398,7 +398,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>7.95662784576416</v>
+        <v>7.934562683105469</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -406,7 +406,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.955420017242432</v>
+        <v>5.874011516571045</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -414,7 +414,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6.767120838165283</v>
+        <v>6.663724422454834</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -422,7 +422,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>7.603854179382324</v>
+        <v>7.561977863311768</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -430,7 +430,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>11.47830581665039</v>
+        <v>11.536208152771</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -438,7 +438,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>13.53664112091064</v>
+        <v>13.69966888427734</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -446,7 +446,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>10.49045848846436</v>
+        <v>10.80807781219482</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -454,7 +454,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4.737107753753662</v>
+        <v>4.527147769927979</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -462,7 +462,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6.079762935638428</v>
+        <v>5.923291206359863</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -470,7 +470,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>4.378615856170654</v>
+        <v>4.451257228851318</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -478,7 +478,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>7.389666080474854</v>
+        <v>7.551928043365479</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -486,7 +486,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>10.40564441680908</v>
+        <v>10.58013725280762</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -494,7 +494,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>10.42655563354492</v>
+        <v>10.74296760559082</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -502,7 +502,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>10.09898853302002</v>
+        <v>10.26916980743408</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -510,7 +510,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>6.089284420013428</v>
+        <v>6.098263263702393</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -518,7 +518,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>4.424148559570312</v>
+        <v>4.29344367980957</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -526,7 +526,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>13.29117012023926</v>
+        <v>13.55679416656494</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -534,7 +534,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>19.33496475219727</v>
+        <v>19.59993553161621</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -542,7 +542,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>6.577813625335693</v>
+        <v>6.560589790344238</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -550,7 +550,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>5.151782989501953</v>
+        <v>5.0816330909729</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -558,7 +558,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>4.395680904388428</v>
+        <v>4.274739742279053</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -566,7 +566,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>6.069608688354492</v>
+        <v>6.05767822265625</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -574,7 +574,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>6.620934963226318</v>
+        <v>6.501260280609131</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -582,7 +582,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>7.318948745727539</v>
+        <v>7.32531213760376</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -590,7 +590,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>11.81636333465576</v>
+        <v>12.09658622741699</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -598,7 +598,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>8.639409065246582</v>
+        <v>8.651673316955566</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -606,7 +606,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>11.24605464935303</v>
+        <v>11.36209487915039</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -614,7 +614,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>14.32633876800537</v>
+        <v>14.84198379516602</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -622,7 +622,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>11.50711727142334</v>
+        <v>11.55424976348877</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -630,7 +630,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>15.95943927764893</v>
+        <v>16.05239677429199</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -638,7 +638,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>6.54820442199707</v>
+        <v>6.340110778808594</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -646,7 +646,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>19.80498123168945</v>
+        <v>19.92737579345703</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -654,7 +654,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>25.43582534790039</v>
+        <v>25.71750259399414</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -662,7 +662,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>13.52932548522949</v>
+        <v>14.04750919342041</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -670,7 +670,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>7.902271747589111</v>
+        <v>7.858399868011475</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -678,7 +678,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>6.021476745605469</v>
+        <v>5.839068412780762</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -686,7 +686,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>6.838600158691406</v>
+        <v>6.640105247497559</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -694,7 +694,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>7.617969036102295</v>
+        <v>7.540596961975098</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -702,7 +702,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>11.15285015106201</v>
+        <v>11.44162750244141</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -710,7 +710,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>13.29177665710449</v>
+        <v>13.59792041778564</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -718,7 +718,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>10.23600673675537</v>
+        <v>10.69638729095459</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -726,7 +726,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>4.950057506561279</v>
+        <v>4.536865234375</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -734,7 +734,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>6.18470287322998</v>
+        <v>5.864860057830811</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -742,7 +742,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>4.31477689743042</v>
+        <v>4.458763122558594</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -750,7 +750,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>7.165870189666748</v>
+        <v>7.484989643096924</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -758,7 +758,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>10.13792991638184</v>
+        <v>10.48827266693115</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -766,7 +766,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>9.974912643432617</v>
+        <v>10.67738342285156</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -774,7 +774,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>9.893525123596191</v>
+        <v>10.18572998046875</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -782,7 +782,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>5.997543811798096</v>
+        <v>6.018743515014648</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -790,7 +790,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>4.566448211669922</v>
+        <v>4.29326868057251</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -798,7 +798,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>12.97424793243408</v>
+        <v>13.44388008117676</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -806,7 +806,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>19.20149993896484</v>
+        <v>19.38541984558105</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -814,7 +814,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>6.523789882659912</v>
+        <v>6.491823196411133</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -822,7 +822,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>5.140477657318115</v>
+        <v>5.036499500274658</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -830,7 +830,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>4.459598064422607</v>
+        <v>4.248396873474121</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -838,7 +838,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>6.025604724884033</v>
+        <v>5.995769500732422</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -846,7 +846,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>6.619915008544922</v>
+        <v>6.410431385040283</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -854,7 +854,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>7.2478346824646</v>
+        <v>7.259796142578125</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -862,7 +862,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>11.04336071014404</v>
+        <v>11.92684364318848</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -870,7 +870,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>8.525527000427246</v>
+        <v>8.585808753967285</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -878,7 +878,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>11.04471969604492</v>
+        <v>11.28206729888916</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -886,7 +886,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>13.73667907714844</v>
+        <v>14.72089862823486</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -894,7 +894,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>11.18331527709961</v>
+        <v>11.45261573791504</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -902,7 +902,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>15.89662742614746</v>
+        <v>15.84002017974854</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -910,7 +910,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>6.532844543457031</v>
+        <v>6.196976661682129</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -918,7 +918,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>19.44545364379883</v>
+        <v>19.68788909912109</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -926,7 +926,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>24.73703193664551</v>
+        <v>25.40290832519531</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -934,7 +934,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>13.4672269821167</v>
+        <v>13.89502143859863</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -942,7 +942,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>7.831560611724854</v>
+        <v>7.770692825317383</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -950,7 +950,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>6.095869064331055</v>
+        <v>5.808511734008789</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -958,7 +958,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>6.864828586578369</v>
+        <v>6.605836868286133</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -966,7 +966,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7.593636989593506</v>
+        <v>7.507067203521729</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -974,7 +974,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>11.05364608764648</v>
+        <v>11.33576107025146</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -982,7 +982,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>13.05564117431641</v>
+        <v>13.48910808563232</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -990,7 +990,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>10.1266508102417</v>
+        <v>10.56950664520264</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -998,7 +998,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>5.177108287811279</v>
+        <v>4.533520221710205</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1006,7 +1006,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>6.270837306976318</v>
+        <v>5.803475379943848</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1014,7 +1014,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>4.252202033996582</v>
+        <v>4.458601474761963</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1022,7 +1022,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>6.946003913879395</v>
+        <v>7.420427799224854</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1030,7 +1030,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>9.864738464355469</v>
+        <v>10.39489078521729</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1038,7 +1038,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>9.410311698913574</v>
+        <v>10.60312271118164</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1046,7 +1046,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>9.71759033203125</v>
+        <v>10.1016731262207</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1054,7 +1054,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>5.906689167022705</v>
+        <v>5.935788631439209</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1062,7 +1062,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>4.805705070495605</v>
+        <v>4.278801918029785</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1070,7 +1070,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>12.64804077148438</v>
+        <v>13.31656265258789</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1078,7 +1078,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>19.15567207336426</v>
+        <v>19.15806579589844</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1086,7 +1086,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>6.473563671112061</v>
+        <v>6.417155742645264</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1094,7 +1094,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>5.091256618499756</v>
+        <v>4.981106281280518</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1102,7 +1102,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>4.499393939971924</v>
+        <v>4.218957424163818</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1110,7 +1110,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>6.052968978881836</v>
+        <v>5.928547859191895</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1118,7 +1118,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>6.607266902923584</v>
+        <v>6.316637992858887</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1126,7 +1126,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>7.175524711608887</v>
+        <v>7.186127662658691</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1134,7 +1134,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>10.60240840911865</v>
+        <v>11.76066780090332</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1142,7 +1142,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>8.40052318572998</v>
+        <v>8.511568069458008</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1150,7 +1150,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>10.70535087585449</v>
+        <v>11.19528484344482</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1158,7 +1158,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>13.24186706542969</v>
+        <v>14.59385108947754</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1166,7 +1166,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>11.0146427154541</v>
+        <v>11.34084892272949</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1174,7 +1174,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>15.82266807556152</v>
+        <v>15.6251916885376</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1182,7 +1182,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>6.48128604888916</v>
+        <v>6.07497501373291</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1190,7 +1190,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>19.08477592468262</v>
+        <v>19.44630241394043</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1198,7 +1198,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>23.96520614624023</v>
+        <v>25.08788681030273</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1206,7 +1206,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>13.74034023284912</v>
+        <v>13.73633766174316</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1214,7 +1214,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7.841311931610107</v>
+        <v>7.671136379241943</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1222,7 +1222,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>6.168068885803223</v>
+        <v>5.777669906616211</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1230,7 +1230,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>6.835846900939941</v>
+        <v>6.559080600738525</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1238,7 +1238,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>7.528514862060547</v>
+        <v>7.459660530090332</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1246,7 +1246,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>10.78582572937012</v>
+        <v>11.21639442443848</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1254,7 +1254,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>12.74608516693115</v>
+        <v>13.36867618560791</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1262,7 +1262,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>10.11339473724365</v>
+        <v>10.42665672302246</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1270,7 +1270,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>5.427739143371582</v>
+        <v>4.514937877655029</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1278,7 +1278,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>6.331255912780762</v>
+        <v>5.735990047454834</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1286,7 +1286,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>4.204568862915039</v>
+        <v>4.447064876556396</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1294,7 +1294,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>6.737100601196289</v>
+        <v>7.355311393737793</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1302,7 +1302,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>9.57958984375</v>
+        <v>10.29762840270996</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1310,7 +1310,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>8.886554718017578</v>
+        <v>10.52012538909912</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1318,7 +1318,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>9.530409812927246</v>
+        <v>10.01451015472412</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1326,7 +1326,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>5.814504623413086</v>
+        <v>5.851010322570801</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1334,7 +1334,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>4.861351013183594</v>
+        <v>4.250696659088135</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1342,7 +1342,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>12.26574897766113</v>
+        <v>13.18251800537109</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1350,7 +1350,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>18.90688514709473</v>
+        <v>18.92146301269531</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1358,7 +1358,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>6.423656940460205</v>
+        <v>6.337779521942139</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1366,7 +1366,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>5.126580238342285</v>
+        <v>4.916608333587646</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1374,7 +1374,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>4.519901275634766</v>
+        <v>4.189223289489746</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1382,7 +1382,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>6.120871543884277</v>
+        <v>5.859615325927734</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1390,7 +1390,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>6.603997707366943</v>
+        <v>6.228358268737793</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1398,7 +1398,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>7.106751918792725</v>
+        <v>7.105429172515869</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1406,7 +1406,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>10.43985939025879</v>
+        <v>11.59707832336426</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1414,7 +1414,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>8.278443336486816</v>
+        <v>8.436002731323242</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1422,7 +1422,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>10.38094711303711</v>
+        <v>11.10911083221436</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1430,7 +1430,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>12.79089641571045</v>
+        <v>14.46375751495361</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1438,7 +1438,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>10.76794719696045</v>
+        <v>11.2252779006958</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1446,7 +1446,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>15.74698162078857</v>
+        <v>15.41115760803223</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1454,7 +1454,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>6.446595668792725</v>
+        <v>5.967560768127441</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1462,7 +1462,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>18.74972724914551</v>
+        <v>19.20959281921387</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1470,7 +1470,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>23.27029037475586</v>
+        <v>24.77530097961426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>